<commit_message>
Team Meeting UPDATED Sep 22, 2021
</commit_message>
<xml_diff>
--- a/Admin/Gaby/TimeSheet_Week5.xlsx
+++ b/Admin/Gaby/TimeSheet_Week5.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">Sponsor Meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TA Meeting</t>
   </si>
   <si>
     <t xml:space="preserve">Organizing (misc.)</t>
@@ -356,10 +359,10 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="6.5"/>
@@ -527,11 +530,11 @@
       <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="B10" s="11"/>
       <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="D10" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="12"/>
@@ -543,45 +546,59 @@
       <c r="J10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="13" t="n">
+      <c r="B11" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="13" t="n">
+        <f aca="false">SUM(B11:H11)</f>
+        <v>1</v>
+      </c>
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="13" t="n">
         <f aca="false">SUM(B6:B9)</f>
         <v>2</v>
       </c>
-      <c r="C11" s="13" t="n">
+      <c r="C12" s="13" t="n">
         <f aca="false">SUM(C6:C9)</f>
         <v>0</v>
       </c>
-      <c r="D11" s="13" t="n">
+      <c r="D12" s="13" t="n">
         <f aca="false">SUM(D6:D9)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="13" t="n">
+      <c r="E12" s="13" t="n">
         <f aca="false">SUM(E6:E9)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="13" t="n">
+      <c r="F12" s="13" t="n">
         <f aca="false">SUM(F6:F9)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="13" t="n">
+      <c r="G12" s="13" t="n">
         <f aca="false">SUM(G6:G9)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="13" t="n">
-        <f aca="false">SUM(H6:H10)</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="13" t="n">
-        <f aca="false">SUM(I6:I10)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
-        <v>13</v>
+      <c r="H12" s="13" t="n">
+        <f aca="false">SUM(H6:H11)</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="13" t="n">
+        <f aca="false">SUM(I6:I11)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -614,7 +631,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Updated Week 5 time sheet
</commit_message>
<xml_diff>
--- a/Admin/Gaby/TimeSheet_Week5.xlsx
+++ b/Admin/Gaby/TimeSheet_Week5.xlsx
@@ -359,10 +359,10 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="6.5"/>
@@ -482,11 +482,15 @@
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="11"/>
+      <c r="G7" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="I7" s="13" t="n">
         <f aca="false">SUM(B7:H7)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J7" s="9"/>
     </row>
@@ -590,15 +594,15 @@
       </c>
       <c r="G12" s="13" t="n">
         <f aca="false">SUM(G6:G9)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="13" t="n">
         <f aca="false">SUM(H6:H11)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="13" t="n">
         <f aca="false">SUM(I6:I11)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Time sheet up to Sep 29.2021
</commit_message>
<xml_diff>
--- a/Admin/Gaby/TimeSheet_Week5.xlsx
+++ b/Admin/Gaby/TimeSheet_Week5.xlsx
@@ -359,10 +359,10 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="6.5"/>
@@ -500,14 +500,16 @@
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="D8" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="12"/>
       <c r="H8" s="11"/>
       <c r="I8" s="13" t="n">
         <f aca="false">SUM(B8:H8)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="9"/>
     </row>
@@ -582,7 +584,7 @@
       </c>
       <c r="D12" s="13" t="n">
         <f aca="false">SUM(D6:D9)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="13" t="n">
         <f aca="false">SUM(E6:E9)</f>
@@ -602,7 +604,7 @@
       </c>
       <c r="I12" s="13" t="n">
         <f aca="false">SUM(I6:I11)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>